<commit_message>
fix squad count exceed the upper limit
</commit_message>
<xml_diff>
--- a/resource/excel/Squad.xlsx
+++ b/resource/excel/Squad.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="14280"/>
+    <workbookView windowHeight="13005" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="SquadData" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="252">
   <si>
     <t>Id</t>
   </si>
@@ -181,7 +181,7 @@
     <t>unit_knight_3_</t>
   </si>
   <si>
-    <t>mal:0</t>
+    <t>mal:100106</t>
   </si>
   <si>
     <t>骑士4</t>
@@ -283,6 +283,9 @@
     <t>ott:16</t>
   </si>
   <si>
+    <t>hre_ha_01:1.6</t>
+  </si>
+  <si>
     <t>火长矛3</t>
   </si>
   <si>
@@ -382,6 +385,9 @@
     <t>unit_horseman_3_</t>
   </si>
   <si>
+    <t>mal</t>
+  </si>
+  <si>
     <t>mal:7.5</t>
   </si>
   <si>
@@ -400,10 +406,10 @@
     <t>unit_ram_3_</t>
   </si>
   <si>
-    <t>冲车钟楼</t>
-  </si>
-  <si>
-    <t>unit_ram_3_clocktower_chi</t>
+    <t>苏丹之塔</t>
+  </si>
+  <si>
+    <t>unit_ram_tower_3_abb_ha_01</t>
   </si>
   <si>
     <t>旗本武士2</t>
@@ -625,9 +631,6 @@
     <t>unit_gbeto_2_</t>
   </si>
   <si>
-    <t>mal</t>
-  </si>
-  <si>
     <t>穆索法迪3</t>
   </si>
   <si>
@@ -745,6 +748,9 @@
     <t>Placeholder</t>
   </si>
   <si>
+    <t>Hide</t>
+  </si>
+  <si>
     <t>Villager</t>
   </si>
   <si>
@@ -763,7 +769,7 @@
     <t>Partial:3</t>
   </si>
   <si>
-    <t>jpn;mon</t>
+    <t>byz;byz</t>
   </si>
   <si>
     <t>#78C8FF;#FD76D8;#7CFF91;#FFFE00</t>
@@ -774,9 +780,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0_ "/>
   </numFmts>
@@ -803,14 +809,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -824,16 +838,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -864,30 +893,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -909,38 +923,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1009,19 +1015,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1033,7 +1051,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1051,37 +1099,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1093,19 +1111,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1117,25 +1129,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1153,31 +1159,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1188,6 +1194,17 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1215,6 +1232,45 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1233,58 +1289,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1296,10 +1302,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1308,133 +1314,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1864,8 +1870,8 @@
   <sheetPr/>
   <dimension ref="A1:R124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D73" workbookViewId="0">
-      <selection activeCell="J112" sqref="J112"/>
+    <sheetView topLeftCell="I16" workbookViewId="0">
+      <selection activeCell="P104" sqref="P104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2314,12 +2320,8 @@
       <c r="L11" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="Q11" t="s">
-        <v>30</v>
-      </c>
-      <c r="R11" t="s">
-        <v>31</v>
-      </c>
+      <c r="Q11"/>
+      <c r="R11"/>
     </row>
     <row r="12" s="7" customFormat="1" spans="1:18">
       <c r="A12" s="12">
@@ -2346,12 +2348,8 @@
         <v>1</v>
       </c>
       <c r="L12" s="9"/>
-      <c r="Q12" t="s">
-        <v>30</v>
-      </c>
-      <c r="R12" t="s">
-        <v>31</v>
-      </c>
+      <c r="Q12"/>
+      <c r="R12"/>
     </row>
     <row r="13" spans="1:18">
       <c r="A13" s="11">
@@ -2439,6 +2437,9 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
       <c r="F15" s="7">
         <f t="shared" si="1"/>
         <v>2.99999997</v>
@@ -2479,6 +2480,9 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
       <c r="F16" s="7">
         <f t="shared" si="1"/>
         <v>3.99999996</v>
@@ -2489,9 +2493,6 @@
       <c r="K16" t="b">
         <v>1</v>
       </c>
-      <c r="L16" s="9" t="s">
-        <v>54</v>
-      </c>
       <c r="Q16" t="s">
         <v>30</v>
       </c>
@@ -2563,15 +2564,15 @@
         <v>61</v>
       </c>
       <c r="C19">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D19" s="7">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F19" s="7">
         <f t="shared" si="1"/>
-        <v>7.99999992</v>
+        <v>9.33333324</v>
       </c>
       <c r="H19">
         <v>200054</v>
@@ -2594,15 +2595,15 @@
         <v>63</v>
       </c>
       <c r="C20">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D20" s="7">
         <f t="shared" ref="D20:D25" si="2">MMULT(C20,1)</f>
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F20" s="7">
         <f t="shared" ref="F20:F25" si="3">MMULT(C20,0.33333333)</f>
-        <v>9.9999999</v>
+        <v>10.66666656</v>
       </c>
       <c r="J20" t="s">
         <v>64</v>
@@ -2629,6 +2630,9 @@
         <f t="shared" si="3"/>
         <v>21.99999978</v>
       </c>
+      <c r="G21">
+        <v>100</v>
+      </c>
       <c r="H21">
         <v>200055</v>
       </c>
@@ -2912,10 +2916,10 @@
         <v>87</v>
       </c>
       <c r="Q30" t="s">
-        <v>31</v>
+        <v>88</v>
       </c>
       <c r="R30" t="s">
-        <v>31</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -2923,7 +2927,7 @@
         <v>100099</v>
       </c>
       <c r="B31" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C31">
         <v>8</v>
@@ -2943,7 +2947,7 @@
         <v>210</v>
       </c>
       <c r="J31" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="K31" t="b">
         <v>0</v>
@@ -2954,7 +2958,7 @@
         <v>200099</v>
       </c>
       <c r="B32" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C32">
         <v>9</v>
@@ -2968,7 +2972,7 @@
         <v>2.99999997</v>
       </c>
       <c r="J32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K32" t="b">
         <v>0</v>
@@ -2979,7 +2983,7 @@
         <v>100100</v>
       </c>
       <c r="B33" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C33">
         <v>47</v>
@@ -3002,7 +3006,7 @@
         <v>540</v>
       </c>
       <c r="J33" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K33" t="b">
         <v>1</v>
@@ -3013,7 +3017,7 @@
         <v>200100</v>
       </c>
       <c r="B34" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C34">
         <v>52</v>
@@ -3036,7 +3040,7 @@
         <v>924</v>
       </c>
       <c r="J34" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K34" t="b">
         <v>0</v>
@@ -3047,7 +3051,7 @@
         <v>300100</v>
       </c>
       <c r="B35" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C35">
         <v>111.6</v>
@@ -3067,7 +3071,7 @@
         <v>0</v>
       </c>
       <c r="J35" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="K35" t="b">
         <v>0</v>
@@ -3078,7 +3082,7 @@
         <v>100101</v>
       </c>
       <c r="B36" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C36">
         <v>63</v>
@@ -3098,7 +3102,7 @@
         <v>580</v>
       </c>
       <c r="J36" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K36" t="b">
         <v>1</v>
@@ -3109,7 +3113,7 @@
         <v>200101</v>
       </c>
       <c r="B37" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C37">
         <v>67</v>
@@ -3123,7 +3127,7 @@
         <v>22.33333311</v>
       </c>
       <c r="J37" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K37" t="b">
         <v>0</v>
@@ -3134,7 +3138,7 @@
         <v>100102</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C38" s="8">
         <v>8</v>
@@ -3154,7 +3158,7 @@
         <v>200</v>
       </c>
       <c r="J38" s="8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="K38" s="8" t="b">
         <v>0</v>
@@ -3166,7 +3170,7 @@
         <v>200102</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C39" s="8">
         <v>10</v>
@@ -3186,7 +3190,7 @@
         <v>290</v>
       </c>
       <c r="J39" s="8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="K39" s="8" t="b">
         <v>0</v>
@@ -3198,7 +3202,7 @@
         <v>300102</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C40" s="8">
         <v>12</v>
@@ -3212,7 +3216,7 @@
         <v>3.99999996</v>
       </c>
       <c r="J40" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="K40" s="8" t="b">
         <v>0</v>
@@ -3224,7 +3228,7 @@
         <v>100103</v>
       </c>
       <c r="B41" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C41">
         <v>25</v>
@@ -3238,7 +3242,7 @@
         <v>8.33333325</v>
       </c>
       <c r="J41" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K41" t="b">
         <v>0</v>
@@ -3249,21 +3253,21 @@
         <v>100104</v>
       </c>
       <c r="B42" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C42">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D42" s="7">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="F42" s="7">
         <f t="shared" si="5"/>
-        <v>8.66666658</v>
+        <v>11.33333322</v>
       </c>
       <c r="J42" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="K42" t="b">
         <v>0</v>
@@ -3274,7 +3278,7 @@
         <v>100105</v>
       </c>
       <c r="B43" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C43">
         <v>6</v>
@@ -3294,7 +3298,7 @@
         <v>220</v>
       </c>
       <c r="J43" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="K43" t="b">
         <v>0</v>
@@ -3305,7 +3309,7 @@
         <v>200105</v>
       </c>
       <c r="B44" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C44">
         <v>8</v>
@@ -3319,7 +3323,7 @@
         <v>2.66666664</v>
       </c>
       <c r="J44" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K44" t="b">
         <v>0</v>
@@ -3330,7 +3334,7 @@
         <v>100106</v>
       </c>
       <c r="B45" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C45">
         <v>5</v>
@@ -3346,6 +3350,9 @@
         <f t="shared" si="5"/>
         <v>1.66666665</v>
       </c>
+      <c r="G45">
+        <v>100</v>
+      </c>
       <c r="H45">
         <v>200106</v>
       </c>
@@ -3353,13 +3360,13 @@
         <v>170</v>
       </c>
       <c r="J45" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="K45" t="b">
         <v>1</v>
       </c>
       <c r="O45" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="Q45" t="s">
         <v>30</v>
@@ -3373,7 +3380,7 @@
         <v>200106</v>
       </c>
       <c r="B46" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C46">
         <v>6</v>
@@ -3396,13 +3403,19 @@
         <v>200</v>
       </c>
       <c r="J46" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="K46" t="b">
         <v>1</v>
       </c>
+      <c r="M46">
+        <v>100052</v>
+      </c>
+      <c r="N46" t="s">
+        <v>122</v>
+      </c>
       <c r="O46" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="Q46" t="s">
         <v>30</v>
@@ -3416,7 +3429,7 @@
         <v>300106</v>
       </c>
       <c r="B47" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C47">
         <v>7</v>
@@ -3433,13 +3446,19 @@
         <v>2.33333331</v>
       </c>
       <c r="J47" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="K47" t="b">
         <v>1</v>
       </c>
+      <c r="M47">
+        <v>200052</v>
+      </c>
+      <c r="N47" t="s">
+        <v>122</v>
+      </c>
       <c r="O47" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="Q47" t="s">
         <v>30</v>
@@ -3453,7 +3472,7 @@
         <v>100107</v>
       </c>
       <c r="B48" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C48">
         <v>30</v>
@@ -3466,11 +3485,14 @@
         <f t="shared" ref="F48:F70" si="6">MMULT(C48,0.33333333)</f>
         <v>9.9999999</v>
       </c>
+      <c r="H48">
+        <v>200107</v>
+      </c>
       <c r="I48">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="J48" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="K48" t="b">
         <v>1</v>
@@ -3481,21 +3503,21 @@
         <v>200107</v>
       </c>
       <c r="B49" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C49">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="D49" s="7">
         <f t="shared" si="4"/>
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="F49" s="7">
         <f t="shared" si="6"/>
-        <v>11.66666655</v>
+        <v>19.9999998</v>
       </c>
       <c r="J49" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="K49" t="b">
         <v>0</v>
@@ -3506,7 +3528,7 @@
         <v>100108</v>
       </c>
       <c r="B50" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C50">
         <v>10</v>
@@ -3526,7 +3548,7 @@
         <v>220</v>
       </c>
       <c r="J50" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="K50" t="b">
         <v>0</v>
@@ -3537,7 +3559,7 @@
         <v>200108</v>
       </c>
       <c r="B51" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C51">
         <v>13</v>
@@ -3557,7 +3579,7 @@
         <v>320</v>
       </c>
       <c r="J51" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="K51" t="b">
         <v>0</v>
@@ -3568,7 +3590,7 @@
         <v>300108</v>
       </c>
       <c r="B52" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C52">
         <v>15</v>
@@ -3582,7 +3604,7 @@
         <v>4.99999995</v>
       </c>
       <c r="J52" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="K52" t="b">
         <v>0</v>
@@ -3593,7 +3615,7 @@
         <v>100109</v>
       </c>
       <c r="B53" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C53">
         <v>8</v>
@@ -3613,7 +3635,7 @@
         <v>200</v>
       </c>
       <c r="J53" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="K53" t="b">
         <v>0</v>
@@ -3624,7 +3646,7 @@
         <v>200109</v>
       </c>
       <c r="B54" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C54">
         <v>11</v>
@@ -3644,7 +3666,7 @@
         <v>300</v>
       </c>
       <c r="J54" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="K54" t="b">
         <v>0</v>
@@ -3655,7 +3677,7 @@
         <v>300109</v>
       </c>
       <c r="B55" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C55">
         <v>12.7</v>
@@ -3669,7 +3691,7 @@
         <v>4.233333291</v>
       </c>
       <c r="J55" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="K55" t="b">
         <v>0</v>
@@ -3680,7 +3702,7 @@
         <v>100110</v>
       </c>
       <c r="B56" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C56">
         <v>9</v>
@@ -3700,7 +3722,7 @@
         <v>230</v>
       </c>
       <c r="J56" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="K56" t="b">
         <v>0</v>
@@ -3711,7 +3733,7 @@
         <v>200110</v>
       </c>
       <c r="B57" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C57">
         <v>11.5</v>
@@ -3731,7 +3753,7 @@
         <v>320</v>
       </c>
       <c r="J57" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="K57" t="b">
         <v>0</v>
@@ -3742,7 +3764,7 @@
         <v>300110</v>
       </c>
       <c r="B58" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C58">
         <v>13</v>
@@ -3756,7 +3778,7 @@
         <v>4.33333329</v>
       </c>
       <c r="J58" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="K58" t="b">
         <v>0</v>
@@ -3767,7 +3789,7 @@
         <v>100111</v>
       </c>
       <c r="B59" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C59">
         <v>6</v>
@@ -3781,7 +3803,7 @@
         <v>1.99999998</v>
       </c>
       <c r="J59" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="K59" t="b">
         <v>0</v>
@@ -3792,7 +3814,7 @@
         <v>100112</v>
       </c>
       <c r="B60" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C60">
         <v>6</v>
@@ -3809,13 +3831,13 @@
         <v>4</v>
       </c>
       <c r="J60" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="K60" t="b">
         <v>0</v>
       </c>
       <c r="L60" s="9" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="61" customFormat="1" spans="1:12">
@@ -3823,7 +3845,7 @@
         <v>100113</v>
       </c>
       <c r="B61" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C61">
         <v>6</v>
@@ -3840,13 +3862,13 @@
         <v>4</v>
       </c>
       <c r="J61" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="K61" t="b">
         <v>0</v>
       </c>
       <c r="L61" s="9" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="62" spans="1:11">
@@ -3854,7 +3876,7 @@
         <v>110001</v>
       </c>
       <c r="B62" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C62">
         <v>80</v>
@@ -3871,7 +3893,7 @@
         <v>1</v>
       </c>
       <c r="J62" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="K62" t="b">
         <v>0</v>
@@ -3882,7 +3904,7 @@
         <v>110002</v>
       </c>
       <c r="B63" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C63">
         <v>100</v>
@@ -3899,7 +3921,7 @@
         <v>2</v>
       </c>
       <c r="J63" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="K63" t="b">
         <v>0</v>
@@ -3910,7 +3932,7 @@
         <v>110003</v>
       </c>
       <c r="B64" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C64">
         <v>9</v>
@@ -3927,7 +3949,7 @@
         <v>1</v>
       </c>
       <c r="J64" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="K64" t="b">
         <v>0</v>
@@ -3938,7 +3960,7 @@
         <v>110004</v>
       </c>
       <c r="B65" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C65">
         <v>19</v>
@@ -3955,7 +3977,7 @@
         <v>1</v>
       </c>
       <c r="J65" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="K65" t="b">
         <v>0</v>
@@ -3997,7 +4019,7 @@
         <v>110006</v>
       </c>
       <c r="B67" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C67">
         <v>12</v>
@@ -4014,7 +4036,7 @@
         <v>1</v>
       </c>
       <c r="J67" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="K67" t="b">
         <v>0</v>
@@ -4025,7 +4047,7 @@
         <v>110007</v>
       </c>
       <c r="B68" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C68">
         <v>120</v>
@@ -4045,7 +4067,7 @@
         <v>2</v>
       </c>
       <c r="J68" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="K68" t="b">
         <v>0</v>
@@ -4056,7 +4078,7 @@
         <v>110008</v>
       </c>
       <c r="B69" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C69">
         <v>140</v>
@@ -4076,7 +4098,7 @@
         <v>2</v>
       </c>
       <c r="J69" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="K69" t="b">
         <v>0</v>
@@ -4087,7 +4109,7 @@
         <v>110009</v>
       </c>
       <c r="B70" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C70">
         <v>6</v>
@@ -4104,7 +4126,7 @@
         <v>1</v>
       </c>
       <c r="J70" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="K70" t="b">
         <v>0</v>
@@ -4115,7 +4137,7 @@
         <v>110010</v>
       </c>
       <c r="B71" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C71">
         <v>16</v>
@@ -4132,7 +4154,7 @@
         <v>1</v>
       </c>
       <c r="J71" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="K71" t="b">
         <v>0</v>
@@ -4143,7 +4165,7 @@
         <v>110011</v>
       </c>
       <c r="B72" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C72">
         <v>26</v>
@@ -4160,7 +4182,7 @@
         <v>1</v>
       </c>
       <c r="J72" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="K72" t="b">
         <v>0</v>
@@ -4171,7 +4193,7 @@
         <v>110012</v>
       </c>
       <c r="B73" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C73">
         <v>19</v>
@@ -4188,7 +4210,7 @@
         <v>1</v>
       </c>
       <c r="J73" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="K73" t="b">
         <v>0</v>
@@ -4216,7 +4238,7 @@
         <v>3</v>
       </c>
       <c r="J74" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="K74" t="b">
         <v>1</v>
@@ -4247,7 +4269,7 @@
         <v>3</v>
       </c>
       <c r="J75" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="K75" t="b">
         <v>1</v>
@@ -4262,7 +4284,7 @@
         <v>210101</v>
       </c>
       <c r="B76" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C76">
         <v>9</v>
@@ -4279,7 +4301,7 @@
         <v>3</v>
       </c>
       <c r="J76" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="K76" t="b">
         <v>1</v>
@@ -4289,7 +4311,7 @@
         <v>100097</v>
       </c>
       <c r="N76" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="77" customFormat="1" spans="1:14">
@@ -4297,18 +4319,18 @@
         <v>210102</v>
       </c>
       <c r="B77" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C77">
-        <v>4.1</v>
+        <v>3.2</v>
       </c>
       <c r="D77" s="7">
         <f t="shared" si="8"/>
-        <v>4.1</v>
+        <v>3.2</v>
       </c>
       <c r="F77" s="7">
         <f t="shared" si="10"/>
-        <v>1.366666653</v>
+        <v>1.066666656</v>
       </c>
       <c r="G77">
         <v>3</v>
@@ -4317,10 +4339,10 @@
         <v>210112</v>
       </c>
       <c r="I77">
-        <v>140</v>
+        <v>90</v>
       </c>
       <c r="J77" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="K77" t="b">
         <v>1</v>
@@ -4330,7 +4352,7 @@
         <v>100050</v>
       </c>
       <c r="N77" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="78" spans="1:14">
@@ -4338,18 +4360,18 @@
         <v>210112</v>
       </c>
       <c r="B78" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C78">
-        <v>5.1</v>
+        <v>4.5</v>
       </c>
       <c r="D78" s="7">
         <f t="shared" si="8"/>
-        <v>5.1</v>
+        <v>4.5</v>
       </c>
       <c r="F78" s="7">
         <f t="shared" si="10"/>
-        <v>1.699999983</v>
+        <v>1.499999985</v>
       </c>
       <c r="G78">
         <v>3</v>
@@ -4358,10 +4380,10 @@
         <v>210122</v>
       </c>
       <c r="I78">
-        <v>220</v>
+        <v>180</v>
       </c>
       <c r="J78" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="K78" t="b">
         <v>1</v>
@@ -4370,7 +4392,7 @@
         <v>200050</v>
       </c>
       <c r="N78" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="79" spans="1:14">
@@ -4378,18 +4400,18 @@
         <v>210122</v>
       </c>
       <c r="B79" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C79">
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="D79" s="7">
         <f t="shared" si="8"/>
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="F79" s="7">
         <f t="shared" si="10"/>
-        <v>1.99999998</v>
+        <v>1.833333315</v>
       </c>
       <c r="G79">
         <v>3</v>
@@ -4398,10 +4420,10 @@
         <v>210132</v>
       </c>
       <c r="I79">
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="J79" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="K79" t="b">
         <v>1</v>
@@ -4410,7 +4432,7 @@
         <v>300050</v>
       </c>
       <c r="N79" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="80" spans="1:14">
@@ -4418,24 +4440,24 @@
         <v>210132</v>
       </c>
       <c r="B80" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C80">
-        <v>6.8</v>
+        <v>6.5</v>
       </c>
       <c r="D80" s="7">
         <f t="shared" si="8"/>
-        <v>6.8</v>
+        <v>6.5</v>
       </c>
       <c r="F80" s="7">
         <f t="shared" si="10"/>
-        <v>2.266666644</v>
+        <v>2.166666645</v>
       </c>
       <c r="G80">
         <v>3</v>
       </c>
       <c r="J80" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="K80" t="b">
         <v>1</v>
@@ -4444,7 +4466,7 @@
         <v>400050</v>
       </c>
       <c r="N80" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="81" spans="1:14">
@@ -4452,7 +4474,7 @@
         <v>210103</v>
       </c>
       <c r="B81" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C81">
         <v>4.9</v>
@@ -4475,7 +4497,7 @@
         <v>180</v>
       </c>
       <c r="J81" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="K81" t="b">
         <v>1</v>
@@ -4484,7 +4506,7 @@
         <v>100051</v>
       </c>
       <c r="N81" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="82" spans="1:14">
@@ -4492,7 +4514,7 @@
         <v>210113</v>
       </c>
       <c r="B82" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C82">
         <v>5.7</v>
@@ -4515,7 +4537,7 @@
         <v>240</v>
       </c>
       <c r="J82" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="K82" t="b">
         <v>1</v>
@@ -4524,7 +4546,7 @@
         <v>200051</v>
       </c>
       <c r="N82" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="83" spans="1:14">
@@ -4532,7 +4554,7 @@
         <v>210123</v>
       </c>
       <c r="B83" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C83">
         <v>6.4</v>
@@ -4549,7 +4571,7 @@
         <v>3</v>
       </c>
       <c r="J83" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="K83" t="b">
         <v>1</v>
@@ -4558,7 +4580,7 @@
         <v>300051</v>
       </c>
       <c r="N83" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="84" customFormat="1" spans="1:14">
@@ -4566,7 +4588,7 @@
         <v>210104</v>
       </c>
       <c r="B84" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C84">
         <v>6.4</v>
@@ -4589,7 +4611,7 @@
         <v>250</v>
       </c>
       <c r="J84" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="K84" t="b">
         <v>1</v>
@@ -4599,7 +4621,7 @@
         <v>100112</v>
       </c>
       <c r="N84" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="85" customFormat="1" spans="1:14">
@@ -4607,7 +4629,7 @@
         <v>210114</v>
       </c>
       <c r="B85" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C85">
         <v>7.2</v>
@@ -4624,7 +4646,7 @@
         <v>3</v>
       </c>
       <c r="J85" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="K85" t="b">
         <v>1</v>
@@ -4634,7 +4656,7 @@
         <v>200112</v>
       </c>
       <c r="N85" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="86" customFormat="1" spans="1:14">
@@ -4642,7 +4664,7 @@
         <v>210105</v>
       </c>
       <c r="B86" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C86">
         <v>4</v>
@@ -4659,7 +4681,7 @@
         <v>3</v>
       </c>
       <c r="J86" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="K86" t="b">
         <v>1</v>
@@ -4669,7 +4691,7 @@
         <v>100113</v>
       </c>
       <c r="N86" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="87" customFormat="1" spans="1:14">
@@ -4677,7 +4699,7 @@
         <v>210201</v>
       </c>
       <c r="B87" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C87">
         <v>110</v>
@@ -4713,7 +4735,7 @@
         <v>100056</v>
       </c>
       <c r="N87" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="88" customFormat="1" spans="1:14">
@@ -4751,7 +4773,7 @@
         <v>200056</v>
       </c>
       <c r="N88" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="89" spans="1:14">
@@ -4759,7 +4781,7 @@
         <v>210301</v>
       </c>
       <c r="B89" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C89">
         <v>4.7</v>
@@ -4782,7 +4804,7 @@
         <v>180</v>
       </c>
       <c r="J89" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="K89" t="b">
         <v>1</v>
@@ -4791,7 +4813,7 @@
         <v>100050</v>
       </c>
       <c r="N89" t="s">
-        <v>202</v>
+        <v>122</v>
       </c>
     </row>
     <row r="90" spans="1:14">
@@ -4799,7 +4821,7 @@
         <v>210311</v>
       </c>
       <c r="B90" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C90">
         <v>5</v>
@@ -4822,7 +4844,7 @@
         <v>210</v>
       </c>
       <c r="J90" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="K90" t="b">
         <v>1</v>
@@ -4831,7 +4853,7 @@
         <v>200050</v>
       </c>
       <c r="N90" t="s">
-        <v>202</v>
+        <v>122</v>
       </c>
     </row>
     <row r="91" spans="1:14">
@@ -4839,7 +4861,7 @@
         <v>210321</v>
       </c>
       <c r="B91" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C91">
         <v>5.4</v>
@@ -4856,7 +4878,7 @@
         <v>3</v>
       </c>
       <c r="J91" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="K91" t="b">
         <v>1</v>
@@ -4865,7 +4887,7 @@
         <v>300050</v>
       </c>
       <c r="N91" t="s">
-        <v>202</v>
+        <v>122</v>
       </c>
     </row>
     <row r="92" spans="1:14">
@@ -4873,7 +4895,7 @@
         <v>210302</v>
       </c>
       <c r="B92" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C92">
         <v>4.7</v>
@@ -4896,7 +4918,7 @@
         <v>160</v>
       </c>
       <c r="J92" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="K92" t="b">
         <v>1</v>
@@ -4905,7 +4927,7 @@
         <v>100051</v>
       </c>
       <c r="N92" t="s">
-        <v>202</v>
+        <v>122</v>
       </c>
     </row>
     <row r="93" spans="1:14">
@@ -4913,7 +4935,7 @@
         <v>210312</v>
       </c>
       <c r="B93" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C93">
         <v>5.7</v>
@@ -4936,7 +4958,7 @@
         <v>220</v>
       </c>
       <c r="J93" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="K93" t="b">
         <v>1</v>
@@ -4945,7 +4967,7 @@
         <v>200051</v>
       </c>
       <c r="N93" t="s">
-        <v>202</v>
+        <v>122</v>
       </c>
     </row>
     <row r="94" spans="1:14">
@@ -4953,7 +4975,7 @@
         <v>210322</v>
       </c>
       <c r="B94" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C94">
         <v>6.7</v>
@@ -4970,7 +4992,7 @@
         <v>3</v>
       </c>
       <c r="J94" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="K94" t="b">
         <v>1</v>
@@ -4979,7 +5001,7 @@
         <v>300051</v>
       </c>
       <c r="N94" t="s">
-        <v>202</v>
+        <v>122</v>
       </c>
     </row>
     <row r="95" customFormat="1" spans="1:14">
@@ -4987,7 +5009,7 @@
         <v>210303</v>
       </c>
       <c r="B95" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C95">
         <v>4</v>
@@ -5010,7 +5032,7 @@
         <v>120</v>
       </c>
       <c r="J95" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="K95" t="b">
         <v>1</v>
@@ -5020,7 +5042,7 @@
         <v>100112</v>
       </c>
       <c r="N95" t="s">
-        <v>202</v>
+        <v>122</v>
       </c>
     </row>
     <row r="96" customFormat="1" spans="1:14">
@@ -5028,7 +5050,7 @@
         <v>210313</v>
       </c>
       <c r="B96" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C96">
         <v>5</v>
@@ -5051,7 +5073,7 @@
         <v>195</v>
       </c>
       <c r="J96" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K96" t="b">
         <v>1</v>
@@ -5061,7 +5083,7 @@
         <v>200112</v>
       </c>
       <c r="N96" t="s">
-        <v>202</v>
+        <v>122</v>
       </c>
     </row>
     <row r="97" customFormat="1" spans="1:14">
@@ -5069,7 +5091,7 @@
         <v>210323</v>
       </c>
       <c r="B97" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C97">
         <v>6.2</v>
@@ -5092,7 +5114,7 @@
         <v>300</v>
       </c>
       <c r="J97" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="K97" t="b">
         <v>1</v>
@@ -5102,7 +5124,7 @@
         <v>300112</v>
       </c>
       <c r="N97" t="s">
-        <v>202</v>
+        <v>122</v>
       </c>
     </row>
     <row r="98" spans="1:14">
@@ -5110,7 +5132,7 @@
         <v>210333</v>
       </c>
       <c r="B98" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C98">
         <v>7.1</v>
@@ -5127,7 +5149,7 @@
         <v>3</v>
       </c>
       <c r="J98" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="K98" t="b">
         <v>1</v>
@@ -5136,7 +5158,7 @@
         <v>400112</v>
       </c>
       <c r="N98" t="s">
-        <v>202</v>
+        <v>122</v>
       </c>
     </row>
     <row r="99" spans="1:14">
@@ -5144,7 +5166,7 @@
         <v>210401</v>
       </c>
       <c r="B99" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C99">
         <v>6.1</v>
@@ -5167,7 +5189,7 @@
         <v>200</v>
       </c>
       <c r="J99" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="K99" t="b">
         <v>1</v>
@@ -5176,7 +5198,7 @@
         <v>100112</v>
       </c>
       <c r="N99" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="100" spans="1:14">
@@ -5184,7 +5206,7 @@
         <v>210411</v>
       </c>
       <c r="B100" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C100">
         <v>7.2</v>
@@ -5207,7 +5229,7 @@
         <v>230</v>
       </c>
       <c r="J100" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="K100" t="b">
         <v>1</v>
@@ -5216,7 +5238,7 @@
         <v>200112</v>
       </c>
       <c r="N100" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="101" spans="1:14">
@@ -5224,7 +5246,7 @@
         <v>210421</v>
       </c>
       <c r="B101" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C101">
         <v>8</v>
@@ -5241,7 +5263,7 @@
         <v>3</v>
       </c>
       <c r="J101" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="K101" t="b">
         <v>1</v>
@@ -5250,7 +5272,7 @@
         <v>300112</v>
       </c>
       <c r="N101" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="102" spans="1:13">
@@ -5275,7 +5297,7 @@
         <v>3</v>
       </c>
       <c r="J102" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="K102" t="b">
         <v>1</v>
@@ -5284,12 +5306,12 @@
         <v>100097</v>
       </c>
     </row>
-    <row r="103" customFormat="1" spans="1:14">
+    <row r="103" customFormat="1" spans="1:18">
       <c r="A103" s="21">
         <v>210601</v>
       </c>
       <c r="B103" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C103">
         <v>5</v>
@@ -5312,7 +5334,7 @@
         <v>200</v>
       </c>
       <c r="J103" s="7" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="K103" t="b">
         <v>1</v>
@@ -5322,10 +5344,16 @@
         <v>100050</v>
       </c>
       <c r="N103" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="104" customFormat="1" spans="1:14">
+        <v>232</v>
+      </c>
+      <c r="Q103" t="s">
+        <v>30</v>
+      </c>
+      <c r="R103" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="104" customFormat="1" spans="1:18">
       <c r="A104" s="21">
         <v>210611</v>
       </c>
@@ -5363,10 +5391,16 @@
         <v>200050</v>
       </c>
       <c r="N104" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="105" customFormat="1" spans="1:14">
+        <v>232</v>
+      </c>
+      <c r="Q104" t="s">
+        <v>30</v>
+      </c>
+      <c r="R104" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="105" customFormat="1" spans="1:18">
       <c r="A105" s="21">
         <v>210621</v>
       </c>
@@ -5398,7 +5432,13 @@
         <v>300050</v>
       </c>
       <c r="N105" t="s">
-        <v>231</v>
+        <v>232</v>
+      </c>
+      <c r="Q105" t="s">
+        <v>30</v>
+      </c>
+      <c r="R105" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="106" customFormat="1" spans="1:14">
@@ -5406,7 +5446,7 @@
         <v>210701</v>
       </c>
       <c r="B106" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C106">
         <v>5.7</v>
@@ -5429,7 +5469,7 @@
         <v>200</v>
       </c>
       <c r="J106" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="K106" t="b">
         <v>1</v>
@@ -5439,7 +5479,7 @@
         <v>100112</v>
       </c>
       <c r="N106" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="107" customFormat="1" spans="1:14">
@@ -5447,7 +5487,7 @@
         <v>210711</v>
       </c>
       <c r="B107" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C107">
         <v>6.2</v>
@@ -5470,7 +5510,7 @@
         <v>245</v>
       </c>
       <c r="J107" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="K107" t="b">
         <v>1</v>
@@ -5480,7 +5520,7 @@
         <v>200112</v>
       </c>
       <c r="N107" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="108" customFormat="1" spans="1:14">
@@ -5488,7 +5528,7 @@
         <v>210721</v>
       </c>
       <c r="B108" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C108">
         <v>7</v>
@@ -5505,7 +5545,7 @@
         <v>3</v>
       </c>
       <c r="J108" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="K108" t="b">
         <v>1</v>
@@ -5515,7 +5555,7 @@
         <v>300112</v>
       </c>
       <c r="N108" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="109" spans="1:1">
@@ -5576,20 +5616,20 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="24.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -5597,7 +5637,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -5605,7 +5645,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -5613,7 +5653,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -5621,10 +5661,18 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B5">
         <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>243</v>
+      </c>
+      <c r="B6">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -5649,22 +5697,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -5678,7 +5726,7 @@
   <sheetPr/>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -5693,7 +5741,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -5701,7 +5749,7 @@
         <v>18</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -5710,7 +5758,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="4" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B4" s="5"/>
     </row>
@@ -5719,7 +5767,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5727,7 +5775,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>